<commit_message>
Mooolya - committing xls, testscript
</commit_message>
<xml_diff>
--- a/src/main/java/com/egp/qa/testdata/EgpTestData.xlsx
+++ b/src/main/java/com/egp/qa/testdata/EgpTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SVN Code Sync\EGP.cptu\src\main\java\com\egp\qa\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shrikanth Kulal\git\Egp.cptu_git\src\main\java\com\egp\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6E33FD-8648-4631-9571-5E4D87F33D14}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A012962E-C15B-40B5-8C70-3F874B25EAEB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AppNewPackageCreation" sheetId="3" r:id="rId1"/>
@@ -247,10 +247,10 @@
     <t>19900002.777</t>
   </si>
   <si>
-    <t>19601122.12</t>
-  </si>
-  <si>
     <t>rokibtenderer13@gmail.com</t>
+  </si>
+  <si>
+    <t>196011254.12</t>
   </si>
 </sst>
 </file>
@@ -816,7 +816,7 @@
       </c>
       <c r="C2" t="str">
         <f ca="1">CELL("filename")</f>
-        <v>D:\SVN Code Sync\EGP.cptu\src\main\java\com\egp\qa\testdata\[EgpTestData.xlsx]appDevptWorkLTMEPW2BTenderLogin</v>
+        <v>C:\Users\Shrikanth Kulal\Desktop\[Bajaj Finance EMI's.xls]Sheet1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1720,7 +1720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40BBEEC-46B9-4EAA-8F76-A5921665410E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="2" spans="1:2" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>46</v>
@@ -1758,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D05769-7033-45B3-B952-36783757C970}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,7 +1877,7 @@
         <v>16</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>22</v>

</xml_diff>